<commit_message>
version fonctionnelle et améliorer pour plusieurs fichiers (laser He-Ne 1 et 2)
</commit_message>
<xml_diff>
--- a/He-Ne_2.xlsx
+++ b/He-Ne_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clément MSI\UL\Session H2024_4\TPOP\Michelson\TPOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0996836E-79DC-46EB-9528-3FF2A61DD92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE461BB5-2907-441F-BC09-9CACF6B199BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,6 +961,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>